<commit_message>
Modification to Benders' main cycle.
</commit_message>
<xml_diff>
--- a/data/HR1/Shared ESS/HR1_ESS.xlsx
+++ b/data/HR1/Shared ESS/HR1_ESS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\shared-resources-planning-v3\data\HR1\Shared ESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1B370F-746B-4034-822F-912448D652C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91790B61-AA1F-48E5-B736-8544150567CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="17640" xr2:uid="{D5815E3E-A825-47B7-91B5-1362E9B2D293}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,10 +484,10 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="D1" s="4">
         <v>0.2</v>
@@ -514,7 +514,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="4">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="D2" s="4">
         <v>1.05</v>
@@ -540,7 +540,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4">
         <v>0.95</v>
@@ -675,15 +675,15 @@
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Winter'!E$2*Scenarios!$C$2</f>
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F2" s="4">
         <f>'Normalized Curves, 2020, Winter'!F$2*Scenarios!$C$2</f>
-        <v>0.57200000000000006</v>
+        <v>0.52</v>
       </c>
       <c r="G2" s="4">
         <f>'Normalized Curves, 2020, Winter'!G$2*Scenarios!$C$2</f>
-        <v>0.49500000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Winter'!H$2*Scenarios!$C$2</f>
@@ -699,15 +699,15 @@
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Winter'!K$2*Scenarios!$C$2</f>
-        <v>0.27500000000000002</v>
+        <v>0.25</v>
       </c>
       <c r="L2" s="4">
         <f>'Normalized Curves, 2020, Winter'!L$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="M2" s="4">
         <f>'Normalized Curves, 2020, Winter'!M$2*Scenarios!$C$2</f>
-        <v>0.38500000000000001</v>
+        <v>0.35</v>
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Winter'!N$2*Scenarios!$C$2</f>
@@ -723,15 +723,15 @@
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Q$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="R2" s="4">
         <f>'Normalized Curves, 2020, Winter'!R$2*Scenarios!$C$2</f>
-        <v>0.38500000000000001</v>
+        <v>0.35</v>
       </c>
       <c r="S2" s="4">
         <f>'Normalized Curves, 2020, Winter'!S$2*Scenarios!$C$2</f>
-        <v>0.45100000000000001</v>
+        <v>0.41</v>
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Winter'!T$2*Scenarios!$C$2</f>
@@ -747,15 +747,15 @@
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Winter'!W$2*Scenarios!$C$2</f>
-        <v>0.16500000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="X2" s="4">
         <f>'Normalized Curves, 2020, Winter'!X$2*Scenarios!$C$2</f>
-        <v>0.16500000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="Y2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Y$2*Scenarios!$C$2</f>
-        <v>0.27500000000000002</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1391,15 +1391,15 @@
       </c>
       <c r="B2" s="4">
         <f>'Normalized Curves, 2020, Summer'!B$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="C2" s="4">
         <f>'Normalized Curves, 2020, Summer'!C$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D2" s="4">
         <f>'Normalized Curves, 2020, Summer'!D$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Summer'!E$3*Scenarios!$C$2</f>
@@ -1415,15 +1415,15 @@
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Summer'!H$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="I2" s="4">
         <f>'Normalized Curves, 2020, Summer'!I$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="J2" s="4">
         <f>'Normalized Curves, 2020, Summer'!J$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Summer'!K$3*Scenarios!$C$2</f>
@@ -1439,15 +1439,15 @@
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Summer'!N$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="O2" s="4">
         <f>'Normalized Curves, 2020, Summer'!O$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="P2" s="4">
         <f>'Normalized Curves, 2020, Summer'!P$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Q$3*Scenarios!$C$2</f>
@@ -1463,15 +1463,15 @@
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Summer'!T$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="U2" s="4">
         <f>'Normalized Curves, 2020, Summer'!U$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="V2" s="4">
         <f>'Normalized Curves, 2020, Summer'!V$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Summer'!W$3*Scenarios!$C$2</f>
@@ -2131,15 +2131,15 @@
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Summer'!E$2*Scenarios!$C$2</f>
-        <v>0.49500000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="F2" s="4">
         <f>'Normalized Curves, 2020, Summer'!F$2*Scenarios!$C$2</f>
-        <v>0.50600000000000012</v>
+        <v>0.46</v>
       </c>
       <c r="G2" s="4">
         <f>'Normalized Curves, 2020, Summer'!G$2*Scenarios!$C$2</f>
-        <v>0.44000000000000006</v>
+        <v>0.4</v>
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Summer'!H$2*Scenarios!$C$2</f>
@@ -2155,15 +2155,15 @@
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Summer'!K$2*Scenarios!$C$2</f>
-        <v>0.31900000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L2" s="4">
         <f>'Normalized Curves, 2020, Summer'!L$2*Scenarios!$C$2</f>
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="M2" s="4">
         <f>'Normalized Curves, 2020, Summer'!M$2*Scenarios!$C$2</f>
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Summer'!N$2*Scenarios!$C$2</f>
@@ -2179,15 +2179,15 @@
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Q$2*Scenarios!$C$2</f>
-        <v>0.30800000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="R2" s="4">
         <f>'Normalized Curves, 2020, Summer'!R$2*Scenarios!$C$2</f>
-        <v>0.30800000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="S2" s="4">
         <f>'Normalized Curves, 2020, Summer'!S$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Summer'!T$2*Scenarios!$C$2</f>
@@ -2203,15 +2203,15 @@
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Summer'!W$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
       <c r="X2" s="4">
         <f>'Normalized Curves, 2020, Summer'!X$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
       <c r="Y2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Y$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2847,15 +2847,15 @@
       </c>
       <c r="B2" s="4">
         <f>'Normalized Curves, 2020, Winter'!B$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="4">
         <f>'Normalized Curves, 2020, Winter'!C$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="D2" s="4">
         <f>'Normalized Curves, 2020, Winter'!D$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Winter'!E$3*Scenarios!$C$2</f>
@@ -2871,15 +2871,15 @@
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Winter'!H$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="I2" s="4">
         <f>'Normalized Curves, 2020, Winter'!I$3*Scenarios!$C$2</f>
-        <v>0.12100000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="J2" s="4">
         <f>'Normalized Curves, 2020, Winter'!J$3*Scenarios!$C$2</f>
-        <v>0.13200000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Winter'!K$3*Scenarios!$C$2</f>
@@ -2895,15 +2895,15 @@
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Winter'!N$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="O2" s="4">
         <f>'Normalized Curves, 2020, Winter'!O$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="P2" s="4">
         <f>'Normalized Curves, 2020, Winter'!P$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Q$3*Scenarios!$C$2</f>
@@ -2919,15 +2919,15 @@
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Winter'!T$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="U2" s="4">
         <f>'Normalized Curves, 2020, Winter'!U$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="V2" s="4">
         <f>'Normalized Curves, 2020, Winter'!V$3*Scenarios!$C$2</f>
-        <v>0.13200000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Winter'!W$3*Scenarios!$C$2</f>
@@ -3587,15 +3587,15 @@
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Winter'!E$2*Scenarios!$C$2</f>
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F2" s="4">
         <f>'Normalized Curves, 2020, Winter'!F$2*Scenarios!$C$2</f>
-        <v>0.57200000000000006</v>
+        <v>0.52</v>
       </c>
       <c r="G2" s="4">
         <f>'Normalized Curves, 2020, Winter'!G$2*Scenarios!$C$2</f>
-        <v>0.49500000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Winter'!H$2*Scenarios!$C$2</f>
@@ -3611,15 +3611,15 @@
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Winter'!K$2*Scenarios!$C$2</f>
-        <v>0.27500000000000002</v>
+        <v>0.25</v>
       </c>
       <c r="L2" s="4">
         <f>'Normalized Curves, 2020, Winter'!L$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="M2" s="4">
         <f>'Normalized Curves, 2020, Winter'!M$2*Scenarios!$C$2</f>
-        <v>0.38500000000000001</v>
+        <v>0.35</v>
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Winter'!N$2*Scenarios!$C$2</f>
@@ -3635,15 +3635,15 @@
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Q$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="R2" s="4">
         <f>'Normalized Curves, 2020, Winter'!R$2*Scenarios!$C$2</f>
-        <v>0.38500000000000001</v>
+        <v>0.35</v>
       </c>
       <c r="S2" s="4">
         <f>'Normalized Curves, 2020, Winter'!S$2*Scenarios!$C$2</f>
-        <v>0.45100000000000001</v>
+        <v>0.41</v>
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Winter'!T$2*Scenarios!$C$2</f>
@@ -3659,15 +3659,15 @@
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Winter'!W$2*Scenarios!$C$2</f>
-        <v>0.16500000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="X2" s="4">
         <f>'Normalized Curves, 2020, Winter'!X$2*Scenarios!$C$2</f>
-        <v>0.16500000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="Y2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Y$2*Scenarios!$C$2</f>
-        <v>0.27500000000000002</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -4303,15 +4303,15 @@
       </c>
       <c r="B2" s="4">
         <f>'Normalized Curves, 2020, Summer'!B$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="C2" s="4">
         <f>'Normalized Curves, 2020, Summer'!C$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D2" s="4">
         <f>'Normalized Curves, 2020, Summer'!D$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Summer'!E$3*Scenarios!$C$2</f>
@@ -4327,15 +4327,15 @@
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Summer'!H$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="I2" s="4">
         <f>'Normalized Curves, 2020, Summer'!I$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="J2" s="4">
         <f>'Normalized Curves, 2020, Summer'!J$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Summer'!K$3*Scenarios!$C$2</f>
@@ -4351,15 +4351,15 @@
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Summer'!N$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="O2" s="4">
         <f>'Normalized Curves, 2020, Summer'!O$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="P2" s="4">
         <f>'Normalized Curves, 2020, Summer'!P$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Q$3*Scenarios!$C$2</f>
@@ -4375,15 +4375,15 @@
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Summer'!T$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="U2" s="4">
         <f>'Normalized Curves, 2020, Summer'!U$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="V2" s="4">
         <f>'Normalized Curves, 2020, Summer'!V$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Summer'!W$3*Scenarios!$C$2</f>
@@ -5043,15 +5043,15 @@
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Summer'!E$2*Scenarios!$C$2</f>
-        <v>0.49500000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="F2" s="4">
         <f>'Normalized Curves, 2020, Summer'!F$2*Scenarios!$C$2</f>
-        <v>0.50600000000000012</v>
+        <v>0.46</v>
       </c>
       <c r="G2" s="4">
         <f>'Normalized Curves, 2020, Summer'!G$2*Scenarios!$C$2</f>
-        <v>0.44000000000000006</v>
+        <v>0.4</v>
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Summer'!H$2*Scenarios!$C$2</f>
@@ -5067,15 +5067,15 @@
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Summer'!K$2*Scenarios!$C$2</f>
-        <v>0.31900000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L2" s="4">
         <f>'Normalized Curves, 2020, Summer'!L$2*Scenarios!$C$2</f>
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="M2" s="4">
         <f>'Normalized Curves, 2020, Summer'!M$2*Scenarios!$C$2</f>
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Summer'!N$2*Scenarios!$C$2</f>
@@ -5091,15 +5091,15 @@
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Q$2*Scenarios!$C$2</f>
-        <v>0.30800000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="R2" s="4">
         <f>'Normalized Curves, 2020, Summer'!R$2*Scenarios!$C$2</f>
-        <v>0.30800000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="S2" s="4">
         <f>'Normalized Curves, 2020, Summer'!S$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Summer'!T$2*Scenarios!$C$2</f>
@@ -5115,15 +5115,15 @@
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Summer'!W$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
       <c r="X2" s="4">
         <f>'Normalized Curves, 2020, Summer'!X$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
       <c r="Y2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Y$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -5759,15 +5759,15 @@
       </c>
       <c r="B2" s="4">
         <f>'Normalized Curves, 2020, Winter'!B$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="4">
         <f>'Normalized Curves, 2020, Winter'!C$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="D2" s="4">
         <f>'Normalized Curves, 2020, Winter'!D$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Winter'!E$3*Scenarios!$C$2</f>
@@ -5783,15 +5783,15 @@
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Winter'!H$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="I2" s="4">
         <f>'Normalized Curves, 2020, Winter'!I$3*Scenarios!$C$2</f>
-        <v>0.12100000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="J2" s="4">
         <f>'Normalized Curves, 2020, Winter'!J$3*Scenarios!$C$2</f>
-        <v>0.13200000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Winter'!K$3*Scenarios!$C$2</f>
@@ -5807,15 +5807,15 @@
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Winter'!N$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="O2" s="4">
         <f>'Normalized Curves, 2020, Winter'!O$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="P2" s="4">
         <f>'Normalized Curves, 2020, Winter'!P$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Q$3*Scenarios!$C$2</f>
@@ -5831,15 +5831,15 @@
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Winter'!T$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="U2" s="4">
         <f>'Normalized Curves, 2020, Winter'!U$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="V2" s="4">
         <f>'Normalized Curves, 2020, Winter'!V$3*Scenarios!$C$2</f>
-        <v>0.13200000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Winter'!W$3*Scenarios!$C$2</f>
@@ -6499,15 +6499,15 @@
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Winter'!E$2*Scenarios!$C$2</f>
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F2" s="4">
         <f>'Normalized Curves, 2020, Winter'!F$2*Scenarios!$C$2</f>
-        <v>0.57200000000000006</v>
+        <v>0.52</v>
       </c>
       <c r="G2" s="4">
         <f>'Normalized Curves, 2020, Winter'!G$2*Scenarios!$C$2</f>
-        <v>0.49500000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Winter'!H$2*Scenarios!$C$2</f>
@@ -6523,15 +6523,15 @@
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Winter'!K$2*Scenarios!$C$2</f>
-        <v>0.27500000000000002</v>
+        <v>0.25</v>
       </c>
       <c r="L2" s="4">
         <f>'Normalized Curves, 2020, Winter'!L$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="M2" s="4">
         <f>'Normalized Curves, 2020, Winter'!M$2*Scenarios!$C$2</f>
-        <v>0.38500000000000001</v>
+        <v>0.35</v>
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Winter'!N$2*Scenarios!$C$2</f>
@@ -6547,15 +6547,15 @@
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Q$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="R2" s="4">
         <f>'Normalized Curves, 2020, Winter'!R$2*Scenarios!$C$2</f>
-        <v>0.38500000000000001</v>
+        <v>0.35</v>
       </c>
       <c r="S2" s="4">
         <f>'Normalized Curves, 2020, Winter'!S$2*Scenarios!$C$2</f>
-        <v>0.45100000000000001</v>
+        <v>0.41</v>
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Winter'!T$2*Scenarios!$C$2</f>
@@ -6571,15 +6571,15 @@
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Winter'!W$2*Scenarios!$C$2</f>
-        <v>0.16500000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="X2" s="4">
         <f>'Normalized Curves, 2020, Winter'!X$2*Scenarios!$C$2</f>
-        <v>0.16500000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="Y2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Y$2*Scenarios!$C$2</f>
-        <v>0.27500000000000002</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -7215,15 +7215,15 @@
       </c>
       <c r="B2" s="4">
         <f>'Normalized Curves, 2020, Summer'!B$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="C2" s="4">
         <f>'Normalized Curves, 2020, Summer'!C$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D2" s="4">
         <f>'Normalized Curves, 2020, Summer'!D$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Summer'!E$3*Scenarios!$C$2</f>
@@ -7239,15 +7239,15 @@
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Summer'!H$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="I2" s="4">
         <f>'Normalized Curves, 2020, Summer'!I$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="J2" s="4">
         <f>'Normalized Curves, 2020, Summer'!J$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Summer'!K$3*Scenarios!$C$2</f>
@@ -7263,15 +7263,15 @@
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Summer'!N$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="O2" s="4">
         <f>'Normalized Curves, 2020, Summer'!O$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="P2" s="4">
         <f>'Normalized Curves, 2020, Summer'!P$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Q$3*Scenarios!$C$2</f>
@@ -7287,15 +7287,15 @@
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Summer'!T$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="U2" s="4">
         <f>'Normalized Curves, 2020, Summer'!U$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="V2" s="4">
         <f>'Normalized Curves, 2020, Summer'!V$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Summer'!W$3*Scenarios!$C$2</f>
@@ -8016,15 +8016,15 @@
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Summer'!E$2*Scenarios!$C$2</f>
-        <v>0.49500000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="F2" s="4">
         <f>'Normalized Curves, 2020, Summer'!F$2*Scenarios!$C$2</f>
-        <v>0.50600000000000012</v>
+        <v>0.46</v>
       </c>
       <c r="G2" s="4">
         <f>'Normalized Curves, 2020, Summer'!G$2*Scenarios!$C$2</f>
-        <v>0.44000000000000006</v>
+        <v>0.4</v>
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Summer'!H$2*Scenarios!$C$2</f>
@@ -8040,15 +8040,15 @@
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Summer'!K$2*Scenarios!$C$2</f>
-        <v>0.31900000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L2" s="4">
         <f>'Normalized Curves, 2020, Summer'!L$2*Scenarios!$C$2</f>
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="M2" s="4">
         <f>'Normalized Curves, 2020, Summer'!M$2*Scenarios!$C$2</f>
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Summer'!N$2*Scenarios!$C$2</f>
@@ -8064,15 +8064,15 @@
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Q$2*Scenarios!$C$2</f>
-        <v>0.30800000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="R2" s="4">
         <f>'Normalized Curves, 2020, Summer'!R$2*Scenarios!$C$2</f>
-        <v>0.30800000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="S2" s="4">
         <f>'Normalized Curves, 2020, Summer'!S$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Summer'!T$2*Scenarios!$C$2</f>
@@ -8088,15 +8088,15 @@
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Summer'!W$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
       <c r="X2" s="4">
         <f>'Normalized Curves, 2020, Summer'!X$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
       <c r="Y2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Y$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -8732,15 +8732,15 @@
       </c>
       <c r="B2" s="4">
         <f>'Normalized Curves, 2020, Winter'!B$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="4">
         <f>'Normalized Curves, 2020, Winter'!C$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="D2" s="4">
         <f>'Normalized Curves, 2020, Winter'!D$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Winter'!E$3*Scenarios!$C$2</f>
@@ -8756,15 +8756,15 @@
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Winter'!H$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="I2" s="4">
         <f>'Normalized Curves, 2020, Winter'!I$3*Scenarios!$C$2</f>
-        <v>0.12100000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="J2" s="4">
         <f>'Normalized Curves, 2020, Winter'!J$3*Scenarios!$C$2</f>
-        <v>0.13200000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Winter'!K$3*Scenarios!$C$2</f>
@@ -8780,15 +8780,15 @@
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Winter'!N$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="O2" s="4">
         <f>'Normalized Curves, 2020, Winter'!O$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="P2" s="4">
         <f>'Normalized Curves, 2020, Winter'!P$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Q$3*Scenarios!$C$2</f>
@@ -8804,15 +8804,15 @@
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Winter'!T$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="U2" s="4">
         <f>'Normalized Curves, 2020, Winter'!U$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="V2" s="4">
         <f>'Normalized Curves, 2020, Winter'!V$3*Scenarios!$C$2</f>
-        <v>0.13200000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Winter'!W$3*Scenarios!$C$2</f>
@@ -9472,15 +9472,15 @@
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Winter'!E$2*Scenarios!$C$2</f>
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F2" s="4">
         <f>'Normalized Curves, 2020, Winter'!F$2*Scenarios!$C$2</f>
-        <v>0.57200000000000006</v>
+        <v>0.52</v>
       </c>
       <c r="G2" s="4">
         <f>'Normalized Curves, 2020, Winter'!G$2*Scenarios!$C$2</f>
-        <v>0.49500000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Winter'!H$2*Scenarios!$C$2</f>
@@ -9496,15 +9496,15 @@
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Winter'!K$2*Scenarios!$C$2</f>
-        <v>0.27500000000000002</v>
+        <v>0.25</v>
       </c>
       <c r="L2" s="4">
         <f>'Normalized Curves, 2020, Winter'!L$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="M2" s="4">
         <f>'Normalized Curves, 2020, Winter'!M$2*Scenarios!$C$2</f>
-        <v>0.38500000000000001</v>
+        <v>0.35</v>
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Winter'!N$2*Scenarios!$C$2</f>
@@ -9520,15 +9520,15 @@
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Q$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="R2" s="4">
         <f>'Normalized Curves, 2020, Winter'!R$2*Scenarios!$C$2</f>
-        <v>0.38500000000000001</v>
+        <v>0.35</v>
       </c>
       <c r="S2" s="4">
         <f>'Normalized Curves, 2020, Winter'!S$2*Scenarios!$C$2</f>
-        <v>0.45100000000000001</v>
+        <v>0.41</v>
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Winter'!T$2*Scenarios!$C$2</f>
@@ -9544,15 +9544,15 @@
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Winter'!W$2*Scenarios!$C$2</f>
-        <v>0.16500000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="X2" s="4">
         <f>'Normalized Curves, 2020, Winter'!X$2*Scenarios!$C$2</f>
-        <v>0.16500000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="Y2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Y$2*Scenarios!$C$2</f>
-        <v>0.27500000000000002</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -10845,15 +10845,15 @@
       </c>
       <c r="B2" s="4">
         <f>'Normalized Curves, 2020, Summer'!B$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="C2" s="4">
         <f>'Normalized Curves, 2020, Summer'!C$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D2" s="4">
         <f>'Normalized Curves, 2020, Summer'!D$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Summer'!E$3*Scenarios!$C$2</f>
@@ -10869,15 +10869,15 @@
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Summer'!H$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="I2" s="4">
         <f>'Normalized Curves, 2020, Summer'!I$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="J2" s="4">
         <f>'Normalized Curves, 2020, Summer'!J$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Summer'!K$3*Scenarios!$C$2</f>
@@ -10893,15 +10893,15 @@
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Summer'!N$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="O2" s="4">
         <f>'Normalized Curves, 2020, Summer'!O$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="P2" s="4">
         <f>'Normalized Curves, 2020, Summer'!P$3*Scenarios!$C$2</f>
-        <v>7.7000000000000013E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Q$3*Scenarios!$C$2</f>
@@ -10917,15 +10917,15 @@
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Summer'!T$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="U2" s="4">
         <f>'Normalized Curves, 2020, Summer'!U$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="V2" s="4">
         <f>'Normalized Curves, 2020, Summer'!V$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Summer'!W$3*Scenarios!$C$2</f>
@@ -11585,15 +11585,15 @@
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Summer'!E$2*Scenarios!$C$2</f>
-        <v>0.49500000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="F2" s="4">
         <f>'Normalized Curves, 2020, Summer'!F$2*Scenarios!$C$2</f>
-        <v>0.50600000000000012</v>
+        <v>0.46</v>
       </c>
       <c r="G2" s="4">
         <f>'Normalized Curves, 2020, Summer'!G$2*Scenarios!$C$2</f>
-        <v>0.44000000000000006</v>
+        <v>0.4</v>
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Summer'!H$2*Scenarios!$C$2</f>
@@ -11609,15 +11609,15 @@
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Summer'!K$2*Scenarios!$C$2</f>
-        <v>0.31900000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L2" s="4">
         <f>'Normalized Curves, 2020, Summer'!L$2*Scenarios!$C$2</f>
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="M2" s="4">
         <f>'Normalized Curves, 2020, Summer'!M$2*Scenarios!$C$2</f>
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Summer'!N$2*Scenarios!$C$2</f>
@@ -11633,15 +11633,15 @@
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Q$2*Scenarios!$C$2</f>
-        <v>0.30800000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="R2" s="4">
         <f>'Normalized Curves, 2020, Summer'!R$2*Scenarios!$C$2</f>
-        <v>0.30800000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="S2" s="4">
         <f>'Normalized Curves, 2020, Summer'!S$2*Scenarios!$C$2</f>
-        <v>0.35200000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Summer'!T$2*Scenarios!$C$2</f>
@@ -11657,15 +11657,15 @@
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Summer'!W$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
       <c r="X2" s="4">
         <f>'Normalized Curves, 2020, Summer'!X$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
       <c r="Y2" s="4">
         <f>'Normalized Curves, 2020, Summer'!Y$2*Scenarios!$C$2</f>
-        <v>0.29700000000000004</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -12301,15 +12301,15 @@
       </c>
       <c r="B2" s="4">
         <f>'Normalized Curves, 2020, Winter'!B$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="4">
         <f>'Normalized Curves, 2020, Winter'!C$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="D2" s="4">
         <f>'Normalized Curves, 2020, Winter'!D$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E2" s="4">
         <f>'Normalized Curves, 2020, Winter'!E$3*Scenarios!$C$2</f>
@@ -12325,15 +12325,15 @@
       </c>
       <c r="H2" s="4">
         <f>'Normalized Curves, 2020, Winter'!H$3*Scenarios!$C$2</f>
-        <v>0.11000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="I2" s="4">
         <f>'Normalized Curves, 2020, Winter'!I$3*Scenarios!$C$2</f>
-        <v>0.12100000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="J2" s="4">
         <f>'Normalized Curves, 2020, Winter'!J$3*Scenarios!$C$2</f>
-        <v>0.13200000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="K2" s="4">
         <f>'Normalized Curves, 2020, Winter'!K$3*Scenarios!$C$2</f>
@@ -12349,15 +12349,15 @@
       </c>
       <c r="N2" s="4">
         <f>'Normalized Curves, 2020, Winter'!N$3*Scenarios!$C$2</f>
-        <v>8.8000000000000009E-2</v>
+        <v>0.08</v>
       </c>
       <c r="O2" s="4">
         <f>'Normalized Curves, 2020, Winter'!O$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="P2" s="4">
         <f>'Normalized Curves, 2020, Winter'!P$3*Scenarios!$C$2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="Q2" s="4">
         <f>'Normalized Curves, 2020, Winter'!Q$3*Scenarios!$C$2</f>
@@ -12373,15 +12373,15 @@
       </c>
       <c r="T2" s="4">
         <f>'Normalized Curves, 2020, Winter'!T$3*Scenarios!$C$2</f>
-        <v>5.5000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="U2" s="4">
         <f>'Normalized Curves, 2020, Winter'!U$3*Scenarios!$C$2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>0.09</v>
       </c>
       <c r="V2" s="4">
         <f>'Normalized Curves, 2020, Winter'!V$3*Scenarios!$C$2</f>
-        <v>0.13200000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="W2" s="4">
         <f>'Normalized Curves, 2020, Winter'!W$3*Scenarios!$C$2</f>

</xml_diff>